<commit_message>
All points from lab work 2 have been completed. It remains to prepare the report.
</commit_message>
<xml_diff>
--- a/Лаба 2/Результаты/Полученные результаты/Обобщённый Вейбула/Сложная гипотеза/Файлы таблиц с данными/Хи-квадрат_result.xlsx
+++ b/Лаба 2/Результаты/Полученные результаты/Обобщённый Вейбула/Сложная гипотеза/Файлы таблиц с данными/Хи-квадрат_result.xlsx
@@ -463,7 +463,7 @@
         <v>500</v>
       </c>
       <c r="C2" t="n">
-        <v>12.2075</v>
+        <v>12.2076</v>
       </c>
       <c r="D2" t="n">
         <v>0.0159</v>
@@ -522,7 +522,7 @@
         <v>1.5667</v>
       </c>
       <c r="D6" t="n">
-        <v>0.8147</v>
+        <v>0.8148</v>
       </c>
     </row>
     <row r="7">

</xml_diff>